<commit_message>
change output caps on local regulators to recommended min
</commit_message>
<xml_diff>
--- a/radiant_v3_bom.xlsx
+++ b/radiant_v3_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Patrick Allison\repositories\github\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2017B3-F8AD-4803-A2DD-D587266C04C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78335484-9960-4814-BF99-BA526AED14E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53854107-050A-4D0C-9425-F001B5382CC3}"/>
   </bookViews>
@@ -2300,22 +2300,22 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10V 0.027uF X7R 0402 10%</t>
   </si>
   <si>
-    <t>C8 C16 C24 C32 C88 C90 C92 C106 C186 C199 C212 C225 C268 C312 C325 C338 C351 C372 C385 C398 C411 C432 C445 C458 C471 CX126 CX128 CX130 CX132 CX134 CX136 CX138 CX140 CX154 CX170 CX186 CX202 CX218 CX234 CX250 CX266 CX282 CX298 CX314 CX330 CX346 CX362 CX378 CX394 CX442 CX446-457 CX477-480 CX490-491 CX496 CX499 CX502-503 CX508-509 CX514-515 CX520-521 CX527-528 CX533-534 CX539-540 CX551</t>
-  </si>
-  <si>
     <t>C273 C504 C583-585</t>
   </si>
   <si>
-    <t>C7 C14 C22 C30 C48 C51 C56 C60 C62 C64 C66 C68 C70 C72-73 C80 C84 C86-87 C89 C91 C93 C95 C97-101 C107-108 C110 C112 C117 C119 C121 C131-132 C134 C136 C148 C150 C161 C163 C171 C173 C177 C182 C184-185 C195 C197-198 C208 C210-211 C221 C223-224 C229 C232 C234-235 C242 C244-245 C253 C261 C298-299 C308 C310-311 C321 C323-324 C334 C336-337 C347 C349-350 C355 C358-359 C368 C370-371 C381 C383-384 C394 C396-397 C407 C409-410 C415 C418-419 C428 C430-431 C441 C443-444 C454 C456-457 C467 C469-470 C475 C502-503 C573-575 CX2-3 CX8-24 CX26-27 CX32-36 CX38-39 CX44-48 CX50-51 CX56-60 CX62 CX64 CX66 CX68-69 CX71-72 CX74-77 CX82 CX84-85 CX90-94 CX96 CX98-99 CX104-108 CX110 CX112-113 CX118-122 CX124-125 CX127 CX129 CX131 CX133 CX135 CX137 CX139 CX142-143 CX145-149 CX153 CX156 CX158-159 CX164-169 CX172 CX174-175 CX180-185 CX188 CX190-191 CX196-201 CX204 CX206-207 CX209-213 CX217 CX220 CX222-223 CX228-233 CX236 CX238-239 CX244-249 CX252 CX254-255 CX260-265 CX268 CX270-271 CX273-277 CX281 CX284 CX286-287 CX292-297 CX300 CX302-303 CX308-313 CX316 CX318-319 CX324-329 CX332 CX334-335 CX337-341 CX345 CX348 CX350-351 CX356-361 CX364 CX366-367 CX372-377 CX380 CX382-383 CX388-393 CX396-436 CX438 CX443-444 CX489 CX552-557</t>
-  </si>
-  <si>
     <t>GRM155R71E223KA61D</t>
   </si>
   <si>
     <t>CAP CER 0.022UF 25V X7R 0402</t>
   </si>
   <si>
-    <t>C2-4 C6 C9-13 C15 C18-21 C23 C26-29 C31 C82 C123-126 C128 C138-142 C144-146 C152-158 C165-169 C179 C188-192 C201-205 C214-218 C231 C255 C263 C301-305 C314-318 C327-331 C340-344 C357 C361-365 C374-378 C387-391 C400-404 C417 C421-425 C434-438 C447-451 C460-464 C477 C576-581 CX437 CX545-550</t>
+    <t>C2-4 C6-7 C9-15 C18-23 C26-31 C82 C87 C89 C91 C93 C123-126 C128 C138-142 C144-146 C152-158 C165-169 C179 C185 C188-192 C198 C201-205 C211 C214-218 C224 C231 C255 C263 C301-305 C311 C314-318 C324 C327-331 C337 C340-344 C350 C357 C361-365 C371 C374-378 C384 C387-391 C397 C400-404 C410 C417 C421-425 C431 C434-438 C444 C447-451 C457 C460-464 C470 C477 C576-581 CX437 CX545-550</t>
+  </si>
+  <si>
+    <t>C8 C16 C24 C32 C88 C90 C92 C106 C186 C199 C212 C225 C268 C312 C325 C338 C351 C372 C385 C398 C411 C432 C445 C458 C471 CX125-140 CX153-154 CX169-170 CX185-186 CX201-202 CX217-218 CX233-234 CX249-250 CX265-266 CX281-282 CX297-298 CX313-314 CX329-330 CX345-346 CX361-362 CX377-378 CX393-394 CX442 CX446-457 CX477-480 CX490-491 CX496 CX499 CX502-503 CX508-509 CX514-515 CX520-521 CX527-528 CX533-534 CX539-540 CX551</t>
+  </si>
+  <si>
+    <t>C48 C51 C56 C60 C62 C64 C66 C68 C70 C72-73 C80 C84 C86 C95 C97-101 C107-108 C110 C112 C117 C119 C121 C131-132 C134 C136 C148 C150 C161 C163 C171 C173 C177 C182 C184 C195 C197 C208 C210 C221 C223 C229 C232 C234-235 C242 C244-245 C253 C261 C298-299 C308 C310 C321 C323 C334 C336 C347 C349 C355 C358-359 C368 C370 C381 C383 C394 C396 C407 C409 C415 C418-419 C428 C430 C441 C443 C454 C456 C467 C469 C475 C502-503 C573-575 CX2-3 CX8-24 CX26-27 CX32-36 CX38-39 CX44-48 CX50-51 CX56-60 CX62 CX64 CX66 CX68-69 CX71-72 CX74-77 CX82 CX84-85 CX90-94 CX96 CX98-99 CX104-108 CX110 CX112-113 CX118-122 CX124 CX142-143 CX145-149 CX156 CX158-159 CX164-168 CX172 CX174-175 CX180-184 CX188 CX190-191 CX196-200 CX204 CX206-207 CX209-213 CX220 CX222-223 CX228-232 CX236 CX238-239 CX244-248 CX252 CX254-255 CX260-264 CX268 CX270-271 CX273-277 CX284 CX286-287 CX292-296 CX300 CX302-303 CX308-312 CX316 CX318-319 CX324-328 CX332 CX334-335 CX337-341 CX348 CX350-351 CX356-360 CX364 CX366-367 CX372-376 CX380 CX382-383 CX388-392 CX396-436 CX438 CX443-444 CX489 CX552-557</t>
   </si>
 </sst>
 </file>
@@ -2690,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84333048-B5AD-486E-BFF9-893CD194EF2A}">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,15 +3169,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="390" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>395</v>
+        <v>347</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="D19" t="s">
         <v>86</v>
@@ -3244,15 +3244,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>99</v>
@@ -3628,10 +3628,10 @@
         <v>131</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3795,10 +3795,10 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>179</v>
@@ -5400,7 +5400,7 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>428</v>
@@ -7199,6 +7199,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update BOM for added feedthrough caps + test points
</commit_message>
<xml_diff>
--- a/radiant_v3_bom.xlsx
+++ b/radiant_v3_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Patrick Allison\repositories\github\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78335484-9960-4814-BF99-BA526AED14E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D84726-73EE-4ABB-9648-C85DDD8D4588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53854107-050A-4D0C-9425-F001B5382CC3}"/>
+    <workbookView xWindow="540" yWindow="1245" windowWidth="22710" windowHeight="12645" xr2:uid="{53854107-050A-4D0C-9425-F001B5382CC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="766">
   <si>
     <t>L15</t>
   </si>
@@ -2316,6 +2316,24 @@
   </si>
   <si>
     <t>C48 C51 C56 C60 C62 C64 C66 C68 C70 C72-73 C80 C84 C86 C95 C97-101 C107-108 C110 C112 C117 C119 C121 C131-132 C134 C136 C148 C150 C161 C163 C171 C173 C177 C182 C184 C195 C197 C208 C210 C221 C223 C229 C232 C234-235 C242 C244-245 C253 C261 C298-299 C308 C310 C321 C323 C334 C336 C347 C349 C355 C358-359 C368 C370 C381 C383 C394 C396 C407 C409 C415 C418-419 C428 C430 C441 C443 C454 C456 C467 C469 C475 C502-503 C573-575 CX2-3 CX8-24 CX26-27 CX32-36 CX38-39 CX44-48 CX50-51 CX56-60 CX62 CX64 CX66 CX68-69 CX71-72 CX74-77 CX82 CX84-85 CX90-94 CX96 CX98-99 CX104-108 CX110 CX112-113 CX118-122 CX124 CX142-143 CX145-149 CX156 CX158-159 CX164-168 CX172 CX174-175 CX180-184 CX188 CX190-191 CX196-200 CX204 CX206-207 CX209-213 CX220 CX222-223 CX228-232 CX236 CX238-239 CX244-248 CX252 CX254-255 CX260-264 CX268 CX270-271 CX273-277 CX284 CX286-287 CX292-296 CX300 CX302-303 CX308-312 CX316 CX318-319 CX324-328 CX332 CX334-335 CX337-341 CX348 CX350-351 CX356-360 CX364 CX366-367 CX372-376 CX380 CX382-383 CX388-392 CX396-436 CX438 CX443-444 CX489 CX552-557</t>
+  </si>
+  <si>
+    <t>C586-609</t>
+  </si>
+  <si>
+    <t>NFM18PC105R0J3D</t>
+  </si>
+  <si>
+    <t>EMIFIL FILTER  NFM18P Murata NFM18C Series, Signal Filter, 6.3 V dc, 2A 0603 SMD 1.6 x 0.8 x 0.8mm</t>
+  </si>
+  <si>
+    <t>TP128-175</t>
+  </si>
+  <si>
+    <t>TESTPOINT_2MM</t>
+  </si>
+  <si>
+    <t>TP_2MM</t>
   </si>
 </sst>
 </file>
@@ -2688,10 +2706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84333048-B5AD-486E-BFF9-893CD194EF2A}">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,25 +5415,25 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>428</v>
+        <v>761</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>429</v>
+        <v>761</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>131</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>430</v>
+        <v>761</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>431</v>
+        <v>762</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5423,25 +5441,25 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>432</v>
+        <v>754</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>435</v>
+        <v>131</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5452,45 +5470,45 @@
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>61</v>
+        <v>435</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>443</v>
+        <v>61</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="H109" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5501,39 +5519,39 @@
         <v>24</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>293</v>
+        <v>443</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>732</v>
+        <v>446</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>293</v>
@@ -5545,122 +5563,122 @@
         <v>450</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>453</v>
+        <v>732</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>237</v>
+        <v>293</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="E114" s="5">
-        <v>603</v>
+        <v>458</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>452</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>452</v>
+        <v>462</v>
+      </c>
+      <c r="E115" s="5">
+        <v>603</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116">
-        <v>224</v>
+        <v>51</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>452</v>
@@ -5669,24 +5687,24 @@
         <v>192</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117">
-        <v>24</v>
+        <v>224</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>452</v>
@@ -5709,10 +5727,10 @@
         <v>24</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>452</v>
@@ -5721,88 +5739,88 @@
         <v>192</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="H118" s="5" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="E120" s="5">
-        <v>603</v>
+        <v>480</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>452</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>485</v>
+        <v>293</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>452</v>
+        <v>484</v>
+      </c>
+      <c r="E121" s="5">
+        <v>603</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>192</v>
+        <v>485</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5813,62 +5831,62 @@
         <v>48</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>452</v>
@@ -5877,10 +5895,10 @@
         <v>192</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5891,22 +5909,22 @@
         <v>1</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H125" s="5" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5914,13 +5932,13 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>452</v>
@@ -5929,10 +5947,10 @@
         <v>293</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H126" s="5" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5940,25 +5958,25 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="H127" s="5" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5966,13 +5984,13 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>452</v>
@@ -5981,36 +5999,36 @@
         <v>192</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H128" s="5" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="E129" s="5">
-        <v>603</v>
+        <v>517</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>452</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>522</v>
+        <v>192</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6018,51 +6036,51 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="E130" s="5" t="s">
-        <v>452</v>
+        <v>521</v>
+      </c>
+      <c r="E130" s="5">
+        <v>603</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>293</v>
+        <v>522</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="H130" s="5" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>531</v>
+        <v>293</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="H131" s="5" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6070,25 +6088,25 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>293</v>
+        <v>531</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6096,25 +6114,25 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -6122,25 +6140,25 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>733</v>
+        <v>540</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>734</v>
+        <v>541</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -6148,25 +6166,25 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>546</v>
+        <v>452</v>
       </c>
       <c r="F135" s="5" t="s">
         <v>293</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>547</v>
+        <v>733</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>548</v>
+        <v>734</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6174,39 +6192,39 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>452</v>
+        <v>546</v>
       </c>
       <c r="F136" s="5" t="s">
         <v>293</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
       <c r="B137">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>452</v>
@@ -6215,36 +6233,36 @@
         <v>293</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6255,74 +6273,74 @@
         <v>1</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="E139" s="5">
-        <v>603</v>
+        <v>558</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>452</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>522</v>
+        <v>192</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H139" s="5" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
       <c r="B140">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="E140" s="5" t="s">
-        <v>452</v>
+        <v>562</v>
+      </c>
+      <c r="E140" s="5">
+        <v>603</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>293</v>
+        <v>522</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="H140" s="5" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
       <c r="B141">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>546</v>
+        <v>452</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -6330,25 +6348,25 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>452</v>
+        <v>546</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -6356,13 +6374,13 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>452</v>
@@ -6371,10 +6389,10 @@
         <v>293</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6382,25 +6400,25 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="H144" s="5" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6411,10 +6429,10 @@
         <v>2</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>452</v>
@@ -6423,85 +6441,85 @@
         <v>192</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
       <c r="B146">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>452</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+      <c r="H146" s="5" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
       <c r="B147">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>593</v>
+        <v>452</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>594</v>
+        <v>10</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="H147" s="5" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
       <c r="B148">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6509,25 +6527,25 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F149" s="5" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6535,19 +6553,25 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>611</v>
+        <v>605</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="G150" s="5" t="s">
+        <v>607</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6558,19 +6582,13 @@
         <v>12</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>610</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="F151" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="G151" s="5" t="s">
-        <v>615</v>
       </c>
       <c r="H151" s="5" t="s">
         <v>612</v>
@@ -6581,25 +6599,25 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="F152" s="5" t="s">
         <v>614</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H152" s="5" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6607,25 +6625,25 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="F153" s="5" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="H153" s="5" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6636,22 +6654,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>735</v>
+        <v>621</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>736</v>
+        <v>622</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>50</v>
+        <v>623</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>51</v>
+        <v>624</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>737</v>
+        <v>625</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6659,48 +6677,48 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>626</v>
+        <v>49</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>627</v>
+        <v>735</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>593</v>
+        <v>736</v>
       </c>
       <c r="F155" s="5" t="s">
-        <v>628</v>
+        <v>50</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H155" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>632</v>
+        <v>593</v>
       </c>
       <c r="F156" s="5" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="G156" s="5" t="s">
-        <v>631</v>
-      </c>
-      <c r="H156" s="5" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6708,51 +6726,51 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="F157" s="5" t="s">
         <v>633</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F158" s="5" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="G158" s="5" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="H158" s="5" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6760,25 +6778,25 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>642</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>600</v>
+        <v>643</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6786,25 +6804,25 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>653</v>
+        <v>600</v>
       </c>
       <c r="G160" s="5" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -6812,25 +6830,25 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="F161" s="5" t="s">
-        <v>10</v>
+        <v>653</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>10</v>
+        <v>654</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6838,77 +6856,77 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F162" s="5" t="s">
-        <v>614</v>
+        <v>10</v>
       </c>
       <c r="G162" s="5" t="s">
-        <v>660</v>
+        <v>10</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>97</v>
+        <v>614</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164">
-        <v>125</v>
+        <v>24</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>10</v>
+        <v>665</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -6916,25 +6934,25 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="F165" s="5" t="s">
-        <v>245</v>
+        <v>10</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>674</v>
+        <v>10</v>
       </c>
       <c r="H165" s="5" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -6942,25 +6960,25 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>676</v>
+        <v>763</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>677</v>
+        <v>764</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>678</v>
+        <v>765</v>
       </c>
       <c r="F166" s="5" t="s">
-        <v>245</v>
+        <v>10</v>
       </c>
       <c r="G166" s="5" t="s">
-        <v>677</v>
+        <v>10</v>
       </c>
       <c r="H166" s="5" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -6971,22 +6989,22 @@
         <v>1</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
       <c r="F167" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="H167" s="5" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -6994,25 +7012,25 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="F168" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -7023,22 +7041,22 @@
         <v>1</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="F169" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -7049,22 +7067,22 @@
         <v>1</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>693</v>
+        <v>681</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>694</v>
+        <v>685</v>
       </c>
       <c r="F170" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G170" s="5" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>696</v>
+        <v>687</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -7075,22 +7093,22 @@
         <v>1</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="F171" s="5" t="s">
-        <v>700</v>
+        <v>245</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>702</v>
+        <v>691</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -7101,22 +7119,22 @@
         <v>1</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>716</v>
+        <v>245</v>
       </c>
       <c r="G172" s="5" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -7127,22 +7145,22 @@
         <v>1</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>709</v>
+        <v>699</v>
       </c>
       <c r="F173" s="5" t="s">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>711</v>
+        <v>701</v>
       </c>
       <c r="H173" s="5" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -7153,22 +7171,22 @@
         <v>1</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>714</v>
+        <v>704</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>715</v>
+        <v>705</v>
       </c>
       <c r="F174" s="5" t="s">
         <v>716</v>
       </c>
       <c r="G174" s="5" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>718</v>
+        <v>706</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -7176,24 +7194,76 @@
         <v>174</v>
       </c>
       <c r="B175">
+        <v>1</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="H175" s="5" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="G176" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
         <v>7</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C177" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D177" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="E175" s="5" t="s">
+      <c r="E177" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="F175" s="5" t="s">
+      <c r="F177" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="G175" s="5" t="s">
+      <c r="G177" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="H175" s="5" t="s">
+      <c r="H177" s="5" t="s">
         <v>723</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update radiant_v3_bom to unify splitter lines
</commit_message>
<xml_diff>
--- a/radiant_v3_bom.xlsx
+++ b/radiant_v3_bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Patrick Allison\repositories\github\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\allison.122\repositories\github\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78335484-9960-4814-BF99-BA526AED14E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04549A97-2A5A-4544-B549-0BF63FE4C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53854107-050A-4D0C-9425-F001B5382CC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{53854107-050A-4D0C-9425-F001B5382CC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="758">
   <si>
     <t>L15</t>
   </si>
@@ -1865,27 +1865,15 @@
     <t>NOR Flash Serial-SPI 3V/3.3V 256M-bit 256M x 1 8ns 24-Pin BGA Tray</t>
   </si>
   <si>
-    <t>T1A T1B T1C T1D T1E T1F T1G T1H T1I T1J T1K T1L</t>
-  </si>
-  <si>
     <t>SBTC-2-10LX+</t>
   </si>
   <si>
     <t>SBTC210LX_6PAD</t>
   </si>
   <si>
-    <t>Signal Conditioning PWR SPLTR CMBD/SM /TOPHAT RoHS</t>
-  </si>
-  <si>
-    <t>T1M T1N T1O T1P T1Q T1R T1S T1T T1U T1V T1W T1X</t>
-  </si>
-  <si>
     <t>Mini-Circuits</t>
   </si>
   <si>
-    <t>TCD-10-1WX+</t>
-  </si>
-  <si>
     <t>T2-7</t>
   </si>
   <si>
@@ -2316,6 +2304,12 @@
   </si>
   <si>
     <t>C48 C51 C56 C60 C62 C64 C66 C68 C70 C72-73 C80 C84 C86 C95 C97-101 C107-108 C110 C112 C117 C119 C121 C131-132 C134 C136 C148 C150 C161 C163 C171 C173 C177 C182 C184 C195 C197 C208 C210 C221 C223 C229 C232 C234-235 C242 C244-245 C253 C261 C298-299 C308 C310 C321 C323 C334 C336 C347 C349 C355 C358-359 C368 C370 C381 C383 C394 C396 C407 C409 C415 C418-419 C428 C430 C441 C443 C454 C456 C467 C469 C475 C502-503 C573-575 CX2-3 CX8-24 CX26-27 CX32-36 CX38-39 CX44-48 CX50-51 CX56-60 CX62 CX64 CX66 CX68-69 CX71-72 CX74-77 CX82 CX84-85 CX90-94 CX96 CX98-99 CX104-108 CX110 CX112-113 CX118-122 CX124 CX142-143 CX145-149 CX156 CX158-159 CX164-168 CX172 CX174-175 CX180-184 CX188 CX190-191 CX196-200 CX204 CX206-207 CX209-213 CX220 CX222-223 CX228-232 CX236 CX238-239 CX244-248 CX252 CX254-255 CX260-264 CX268 CX270-271 CX273-277 CX284 CX286-287 CX292-296 CX300 CX302-303 CX308-312 CX316 CX318-319 CX324-328 CX332 CX334-335 CX337-341 CX348 CX350-351 CX356-360 CX364 CX366-367 CX372-376 CX380 CX382-383 CX388-392 CX396-436 CX438 CX443-444 CX489 CX552-557</t>
+  </si>
+  <si>
+    <t>T1A T1B T1C T1D T1E T1F T1G T1H T1I T1J T1K T1L T1M T1N T1O T1P T1Q T1R T1S T1T T1U T1V T1W T1X</t>
+  </si>
+  <si>
+    <t>Signal Conditioning PWR SPLTR CMBD/SM /TOPHAT RoHS: NOTE - pin 5 is NOT PRESENT in this variant</t>
   </si>
 </sst>
 </file>
@@ -2688,49 +2682,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84333048-B5AD-486E-BFF9-893CD194EF2A}">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="48.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="106.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="106.33203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>742</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>743</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>744</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2753,10 +2747,10 @@
         <v>744314330</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2782,7 +2776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2805,7 +2799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2831,7 +2825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2857,7 +2851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2883,7 +2877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2909,7 +2903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2935,7 +2929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2961,7 +2955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2987,7 +2981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3013,7 +3007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3039,7 +3033,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3065,7 +3059,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3091,7 +3085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3117,7 +3111,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3137,13 +3131,13 @@
         <v>79</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3169,7 +3163,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3177,7 +3171,7 @@
         <v>347</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="D19" t="s">
         <v>86</v>
@@ -3195,7 +3189,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3221,7 +3215,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3244,7 +3238,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3252,7 +3246,7 @@
         <v>165</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>99</v>
@@ -3270,7 +3264,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3296,7 +3290,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3322,7 +3316,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3348,7 +3342,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3356,7 +3350,7 @@
         <v>223</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>115</v>
@@ -3368,13 +3362,13 @@
         <v>131</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3400,7 +3394,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3426,7 +3420,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3452,7 +3446,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3478,7 +3472,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3504,7 +3498,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3530,7 +3524,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3556,7 +3550,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3582,7 +3576,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3608,7 +3602,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3628,13 +3622,13 @@
         <v>131</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3660,7 +3654,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3680,13 +3674,13 @@
         <v>88</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3694,7 +3688,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>164</v>
@@ -3712,7 +3706,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3738,7 +3732,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3764,7 +3758,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3790,7 +3784,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3798,7 +3792,7 @@
         <v>109</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>179</v>
@@ -3816,7 +3810,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3842,7 +3836,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3868,7 +3862,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3894,7 +3888,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3920,7 +3914,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3928,25 +3922,25 @@
         <v>3</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>200</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>83</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3972,7 +3966,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3998,7 +3992,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4024,7 +4018,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4032,7 +4026,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>212</v>
@@ -4050,7 +4044,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4076,7 +4070,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4102,7 +4096,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4128,7 +4122,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4154,7 +4148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4180,7 +4174,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4206,7 +4200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4226,13 +4220,13 @@
         <v>116</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4258,7 +4252,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4284,7 +4278,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4310,7 +4304,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4336,7 +4330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4362,7 +4356,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4388,7 +4382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4411,7 +4405,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4434,7 +4428,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4460,7 +4454,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4486,7 +4480,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4509,7 +4503,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4535,7 +4529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4555,7 +4549,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4575,7 +4569,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4601,7 +4595,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4624,7 +4618,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4647,7 +4641,7 @@
         <v>744917215</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4670,7 +4664,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4696,7 +4690,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4722,7 +4716,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4748,7 +4742,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4774,7 +4768,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4800,7 +4794,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4826,7 +4820,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4852,7 +4846,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4878,7 +4872,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4904,7 +4898,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4930,7 +4924,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4956,7 +4950,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4982,7 +4976,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5008,7 +5002,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5034,7 +5028,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5060,7 +5054,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5083,7 +5077,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5109,7 +5103,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5135,7 +5129,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5161,7 +5155,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5187,7 +5181,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5213,7 +5207,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5236,7 +5230,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5262,7 +5256,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5288,7 +5282,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5314,7 +5308,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5340,7 +5334,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5366,7 +5360,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5392,7 +5386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5400,7 +5394,7 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>428</v>
@@ -5418,7 +5412,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5444,7 +5438,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5467,7 +5461,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5493,7 +5487,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5519,7 +5513,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5527,7 +5521,7 @@
         <v>54</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>451</v>
@@ -5545,7 +5539,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5571,7 +5565,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5597,7 +5591,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5623,7 +5617,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5649,7 +5643,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5675,7 +5669,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5701,7 +5695,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5727,7 +5721,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5753,7 +5747,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5779,7 +5773,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5805,7 +5799,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5831,7 +5825,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5857,7 +5851,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5883,7 +5877,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5909,7 +5903,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5935,7 +5929,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5961,7 +5955,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5987,7 +5981,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6013,7 +6007,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6039,7 +6033,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -6065,7 +6059,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -6091,7 +6085,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -6117,7 +6111,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -6137,13 +6131,13 @@
         <v>293</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -6169,7 +6163,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -6195,7 +6189,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -6221,7 +6215,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -6247,7 +6241,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -6273,7 +6267,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -6299,7 +6293,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -6325,7 +6319,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -6351,7 +6345,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -6377,7 +6371,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -6403,7 +6397,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6429,7 +6423,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6452,7 +6446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6478,7 +6472,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6504,7 +6498,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6530,58 +6524,64 @@
         <v>608</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
       <c r="B150">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D150" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="E150" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="E150" s="5" t="s">
+      <c r="F150" s="5" t="s">
         <v>611</v>
       </c>
+      <c r="G150" s="5" t="s">
+        <v>609</v>
+      </c>
       <c r="H150" s="5" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
       <c r="B151">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D151" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="D151" s="5" t="s">
-        <v>610</v>
-      </c>
       <c r="E151" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="F151" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="F151" s="5" t="s">
-        <v>614</v>
-      </c>
       <c r="G151" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="H151" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="H151" s="5" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
       <c r="B152">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>616</v>
@@ -6593,16 +6593,16 @@
         <v>618</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="H152" s="5" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6610,56 +6610,53 @@
         <v>1</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>620</v>
+        <v>49</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>621</v>
+        <v>731</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>622</v>
+        <v>732</v>
       </c>
       <c r="F153" s="5" t="s">
-        <v>623</v>
+        <v>50</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>624</v>
+        <v>51</v>
       </c>
       <c r="H153" s="5" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>49</v>
+        <v>622</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>735</v>
+        <v>623</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>736</v>
+        <v>593</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>50</v>
+        <v>624</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H154" s="5" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>626</v>
@@ -6668,85 +6665,88 @@
         <v>627</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>593</v>
+        <v>628</v>
       </c>
       <c r="F155" s="5" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+      <c r="H155" s="5" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F156" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="G156" s="5" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="H156" s="5" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F157" s="5" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="F158" s="5" t="s">
-        <v>643</v>
+        <v>600</v>
       </c>
       <c r="G158" s="5" t="s">
         <v>644</v>
@@ -6755,12 +6755,12 @@
         <v>645</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
       <c r="B159">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>646</v>
@@ -6769,76 +6769,76 @@
         <v>647</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>600</v>
+        <v>649</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>653</v>
+        <v>10</v>
       </c>
       <c r="G160" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H160" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="H160" s="5" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C161" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D161" s="5" t="s">
         <v>656</v>
-      </c>
-      <c r="D161" s="5" t="s">
-        <v>657</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>657</v>
       </c>
       <c r="F161" s="5" t="s">
-        <v>10</v>
+        <v>611</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>10</v>
+        <v>656</v>
       </c>
       <c r="H161" s="5" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>659</v>
@@ -6847,24 +6847,24 @@
         <v>660</v>
       </c>
       <c r="E162" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G162" s="5" t="s">
         <v>661</v>
-      </c>
-      <c r="F162" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>660</v>
       </c>
       <c r="H162" s="5" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>663</v>
@@ -6873,24 +6873,24 @@
         <v>664</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>665</v>
+        <v>10</v>
       </c>
       <c r="H163" s="5" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>667</v>
@@ -6902,47 +6902,47 @@
         <v>669</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>10</v>
+        <v>245</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>10</v>
+        <v>670</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F165" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H165" s="5" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>676</v>
@@ -6963,7 +6963,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6974,22 +6974,22 @@
         <v>680</v>
       </c>
       <c r="D167" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="E167" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E167" s="5" t="s">
-        <v>682</v>
       </c>
       <c r="F167" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -7000,22 +7000,22 @@
         <v>684</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F168" s="5" t="s">
         <v>245</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H168" s="5" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -7035,13 +7035,13 @@
         <v>245</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -7049,25 +7049,25 @@
         <v>1</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="F170" s="5" t="s">
-        <v>245</v>
+        <v>696</v>
       </c>
       <c r="G170" s="5" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -7075,25 +7075,25 @@
         <v>1</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="F171" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="G171" s="5" t="s">
         <v>700</v>
-      </c>
-      <c r="G171" s="5" t="s">
-        <v>701</v>
       </c>
       <c r="H171" s="5" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -7110,16 +7110,16 @@
         <v>705</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>716</v>
+        <v>706</v>
       </c>
       <c r="G172" s="5" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -7127,74 +7127,48 @@
         <v>1</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="F173" s="5" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="H173" s="5" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="F174" s="5" t="s">
-        <v>716</v>
+        <v>245</v>
       </c>
       <c r="G174" s="5" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>174</v>
-      </c>
-      <c r="B175">
-        <v>7</v>
-      </c>
-      <c r="C175" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="D175" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="E175" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="F175" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="G175" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="H175" s="5" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>